<commit_message>
Update the metadata templates.
</commit_message>
<xml_diff>
--- a/public/metadata-templates/genomics-metadata-template.xlsx
+++ b/public/metadata-templates/genomics-metadata-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/choppy/Documents/Code/ChineseQuartet/quartet-studio/public/metadata-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E28576-8963-D54D-B9E6-B85757B5EC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE6AADB-E40F-4B43-A807-57CEAEA6F05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="16300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>The format of an electronic file.</t>
+  </si>
+  <si>
+    <t>You need to rename the excel file to metadata.xlsx before you uploading to Quartet Data Portal.</t>
   </si>
   <si>
     <r>
@@ -197,11 +200,8 @@
         <rFont val="Arial Regular"/>
       </rPr>
       <t xml:space="preserve"> 
-NOTE: This template table may change in the future as the specification is upgraded</t>
+NOTE: This template table may change in the future as the specification is upgraded. (Current Version: 20220505)</t>
     </r>
-  </si>
-  <si>
-    <t>You need to rename the excel file to metadata.xlsx before you uploading to Quartet Data Portal.</t>
   </si>
 </sst>
 </file>
@@ -683,7 +683,7 @@
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="23" defaultRowHeight="23" customHeight="1"/>
@@ -709,7 +709,7 @@
     </row>
     <row r="2" spans="1:7" ht="36" customHeight="1">
       <c r="A2" s="28" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
@@ -720,7 +720,7 @@
     </row>
     <row r="3" spans="1:7" ht="23" customHeight="1">
       <c r="A3" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
@@ -1350,7 +1350,7 @@
       <c r="E69" s="10"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qI7tADcO6tJpKYSqT1PRmtmPZdZpfFBykzE09KecRtizyBfk7/1x0ACFZzHI2Cq57K6XZQK2cklvgRCm4Kr6Dg==" saltValue="DNZTznbHMHBrV6n5gZ5HPQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="QjIECM+fa+pg1XnLU2tKn3iccJh43qWaX+5Pmw8qw28LDMhqZo1sHPnUyMA9yFa3+7KzY9CtdcJ4GWzwLXujVQ==" saltValue="DDGQ6uI0LtsPZSK21+h8Vw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>

</xml_diff>